<commit_message>
Test! 3 market, 3 oper, 5 years.
</commit_message>
<xml_diff>
--- a/data/CS7/Market Data/CS7_market_data_2030.xlsx
+++ b/data/CS7/Market Data/CS7_market_data_2030.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS7\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263378DF-A8A2-498D-918F-9B67D9157E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025334DD-F40B-4372-B273-1B8119A09CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-12555" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -2242,19 +2242,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>